<commit_message>
:whale: Docker django-postgresql funcionando
</commit_message>
<xml_diff>
--- a/resultado.xlsx
+++ b/resultado.xlsx
@@ -505,7 +505,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>covid_vacuna</t>
+          <t>covid_vacunado</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -2312,13 +2312,13 @@
       <c r="K2" t="n">
         <v>23</v>
       </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2" t="b">
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
         <v>1</v>
       </c>
       <c r="O2" t="inlineStr">
@@ -2326,22 +2326,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S2" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U2" t="b">
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
       <c r="V2" t="n">
@@ -3509,13 +3513,13 @@
       <c r="K3" t="n">
         <v>18</v>
       </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N3" t="b">
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
         <v>1</v>
       </c>
       <c r="O3" t="inlineStr">
@@ -3523,22 +3527,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S3" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T3" t="b">
-        <v>1</v>
-      </c>
-      <c r="U3" t="b">
+      <c r="T3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" t="n">
         <v>0</v>
       </c>
       <c r="V3" t="n">
@@ -4706,13 +4714,13 @@
       <c r="K4" t="n">
         <v>19</v>
       </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N4" t="b">
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
         <v>1</v>
       </c>
       <c r="O4" t="inlineStr">
@@ -4720,22 +4728,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S4" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T4" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" t="b">
+      <c r="T4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" t="n">
         <v>0</v>
       </c>
       <c r="V4" t="n">
@@ -5903,13 +5915,13 @@
       <c r="K5" t="n">
         <v>21</v>
       </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" t="b">
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
         <v>1</v>
       </c>
       <c r="O5" t="inlineStr">
@@ -5917,22 +5929,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S5" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U5" t="b">
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
         <v>0</v>
       </c>
       <c r="V5" t="n">
@@ -7100,13 +7116,13 @@
       <c r="K6" t="n">
         <v>18</v>
       </c>
-      <c r="L6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" t="b">
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
         <v>1</v>
       </c>
       <c r="O6" t="inlineStr">
@@ -7114,22 +7130,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S6" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" t="b">
+      <c r="T6" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" t="n">
         <v>0</v>
       </c>
       <c r="V6" t="n">
@@ -8297,13 +8317,13 @@
       <c r="K7" t="n">
         <v>19</v>
       </c>
-      <c r="L7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" t="b">
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
         <v>1</v>
       </c>
       <c r="O7" t="inlineStr">
@@ -8311,22 +8331,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
-      </c>
-      <c r="R7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S7" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T7" t="b">
-        <v>1</v>
-      </c>
-      <c r="U7" t="b">
+      <c r="T7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U7" t="n">
         <v>0</v>
       </c>
       <c r="V7" t="n">
@@ -9494,13 +9518,13 @@
       <c r="K8" t="n">
         <v>21</v>
       </c>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8" t="b">
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
         <v>1</v>
       </c>
       <c r="O8" t="inlineStr">
@@ -9508,22 +9532,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P8" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="b">
-        <v>0</v>
-      </c>
-      <c r="R8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S8" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T8" t="b">
-        <v>1</v>
-      </c>
-      <c r="U8" t="b">
+      <c r="T8" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" t="n">
         <v>0</v>
       </c>
       <c r="V8" t="n">
@@ -10691,13 +10719,13 @@
       <c r="K9" t="n">
         <v>22</v>
       </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" t="b">
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
         <v>1</v>
       </c>
       <c r="O9" t="inlineStr">
@@ -10705,22 +10733,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S9" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T9" t="b">
-        <v>1</v>
-      </c>
-      <c r="U9" t="b">
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" t="n">
         <v>0</v>
       </c>
       <c r="V9" t="n">
@@ -11888,13 +11920,13 @@
       <c r="K10" t="n">
         <v>20</v>
       </c>
-      <c r="L10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" t="b">
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
         <v>1</v>
       </c>
       <c r="O10" t="inlineStr">
@@ -11902,22 +11934,26 @@
           <t>M</t>
         </is>
       </c>
-      <c r="P10" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q10" t="b">
-        <v>0</v>
-      </c>
-      <c r="R10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S10" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T10" t="b">
-        <v>1</v>
-      </c>
-      <c r="U10" t="b">
+      <c r="T10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U10" t="n">
         <v>0</v>
       </c>
       <c r="V10" t="n">
@@ -13085,13 +13121,13 @@
       <c r="K11" t="n">
         <v>21</v>
       </c>
-      <c r="L11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" t="b">
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
         <v>1</v>
       </c>
       <c r="O11" t="inlineStr">
@@ -13099,22 +13135,26 @@
           <t>J</t>
         </is>
       </c>
-      <c r="P11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="b">
-        <v>0</v>
-      </c>
-      <c r="R11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S11" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T11" t="b">
-        <v>1</v>
-      </c>
-      <c r="U11" t="b">
+      <c r="T11" t="n">
+        <v>1</v>
+      </c>
+      <c r="U11" t="n">
         <v>0</v>
       </c>
       <c r="V11" t="n">
@@ -14282,13 +14322,13 @@
       <c r="K12" t="n">
         <v>19</v>
       </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
         <v>1</v>
       </c>
       <c r="O12" t="inlineStr">
@@ -14296,22 +14336,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>0</v>
-      </c>
-      <c r="R12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T12" t="b">
-        <v>1</v>
-      </c>
-      <c r="U12" t="b">
+      <c r="T12" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" t="n">
         <v>0</v>
       </c>
       <c r="V12" t="n">
@@ -15479,13 +15523,13 @@
       <c r="K13" t="n">
         <v>22</v>
       </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" t="b">
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
         <v>1</v>
       </c>
       <c r="O13" t="inlineStr">
@@ -15493,22 +15537,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q13" t="b">
-        <v>0</v>
-      </c>
-      <c r="R13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S13" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T13" t="b">
-        <v>1</v>
-      </c>
-      <c r="U13" t="b">
+      <c r="T13" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" t="n">
         <v>0</v>
       </c>
       <c r="V13" t="n">
@@ -16676,13 +16724,13 @@
       <c r="K14" t="n">
         <v>21</v>
       </c>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" t="b">
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="inlineStr">
@@ -16690,22 +16738,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P14" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q14" t="b">
-        <v>0</v>
-      </c>
-      <c r="R14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S14" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T14" t="b">
-        <v>1</v>
-      </c>
-      <c r="U14" t="b">
+      <c r="T14" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" t="n">
         <v>0</v>
       </c>
       <c r="V14" t="n">
@@ -17873,13 +17925,13 @@
       <c r="K15" t="n">
         <v>23</v>
       </c>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-      <c r="M15" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" t="b">
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
         <v>1</v>
       </c>
       <c r="O15" t="inlineStr">
@@ -17887,22 +17939,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P15" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="b">
-        <v>0</v>
-      </c>
-      <c r="R15" t="inlineStr"/>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S15" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T15" t="b">
-        <v>1</v>
-      </c>
-      <c r="U15" t="b">
+      <c r="T15" t="n">
+        <v>1</v>
+      </c>
+      <c r="U15" t="n">
         <v>0</v>
       </c>
       <c r="V15" t="n">
@@ -19070,13 +19126,13 @@
       <c r="K16" t="n">
         <v>21</v>
       </c>
-      <c r="L16" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" t="b">
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
         <v>1</v>
       </c>
       <c r="O16" t="inlineStr">
@@ -19084,22 +19140,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="b">
-        <v>0</v>
-      </c>
-      <c r="R16" t="inlineStr"/>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S16" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T16" t="b">
-        <v>1</v>
-      </c>
-      <c r="U16" t="b">
+      <c r="T16" t="n">
+        <v>1</v>
+      </c>
+      <c r="U16" t="n">
         <v>0</v>
       </c>
       <c r="V16" t="n">
@@ -20267,13 +20327,13 @@
       <c r="K17" t="n">
         <v>21</v>
       </c>
-      <c r="L17" t="b">
-        <v>1</v>
-      </c>
-      <c r="M17" t="b">
-        <v>1</v>
-      </c>
-      <c r="N17" t="b">
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" t="n">
         <v>1</v>
       </c>
       <c r="O17" t="inlineStr">
@@ -20281,22 +20341,26 @@
           <t>J</t>
         </is>
       </c>
-      <c r="P17" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="b">
-        <v>0</v>
-      </c>
-      <c r="R17" t="inlineStr"/>
+      <c r="P17" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S17" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T17" t="b">
-        <v>1</v>
-      </c>
-      <c r="U17" t="b">
+      <c r="T17" t="n">
+        <v>1</v>
+      </c>
+      <c r="U17" t="n">
         <v>0</v>
       </c>
       <c r="V17" t="n">
@@ -21464,13 +21528,13 @@
       <c r="K18" t="n">
         <v>20</v>
       </c>
-      <c r="L18" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" t="b">
-        <v>1</v>
-      </c>
-      <c r="N18" t="b">
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" t="n">
         <v>1</v>
       </c>
       <c r="O18" t="inlineStr">
@@ -21478,10 +21542,10 @@
           <t>J</t>
         </is>
       </c>
-      <c r="P18" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="b">
+      <c r="P18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="n">
         <v>0</v>
       </c>
       <c r="R18" t="inlineStr"/>
@@ -21490,10 +21554,10 @@
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T18" t="b">
-        <v>1</v>
-      </c>
-      <c r="U18" t="b">
+      <c r="T18" t="n">
+        <v>1</v>
+      </c>
+      <c r="U18" t="n">
         <v>0</v>
       </c>
       <c r="V18" t="n">
@@ -22661,13 +22725,13 @@
       <c r="K19" t="n">
         <v>21</v>
       </c>
-      <c r="L19" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" t="b">
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
         <v>1</v>
       </c>
       <c r="O19" t="inlineStr">
@@ -22675,22 +22739,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P19" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="b">
-        <v>0</v>
-      </c>
-      <c r="R19" t="inlineStr"/>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S19" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T19" t="b">
-        <v>1</v>
-      </c>
-      <c r="U19" t="b">
+      <c r="T19" t="n">
+        <v>1</v>
+      </c>
+      <c r="U19" t="n">
         <v>0</v>
       </c>
       <c r="V19" t="n">
@@ -23858,13 +23926,13 @@
       <c r="K20" t="n">
         <v>23</v>
       </c>
-      <c r="L20" t="b">
-        <v>1</v>
-      </c>
-      <c r="M20" t="b">
-        <v>1</v>
-      </c>
-      <c r="N20" t="b">
+      <c r="L20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" t="n">
         <v>1</v>
       </c>
       <c r="O20" t="inlineStr">
@@ -23872,22 +23940,26 @@
           <t>J</t>
         </is>
       </c>
-      <c r="P20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q20" t="b">
-        <v>0</v>
-      </c>
-      <c r="R20" t="inlineStr"/>
+      <c r="P20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S20" t="inlineStr">
         <is>
           <t>Practicante en Montechelo Technology</t>
         </is>
       </c>
-      <c r="T20" t="b">
-        <v>0</v>
-      </c>
-      <c r="U20" t="b">
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
         <v>0</v>
       </c>
       <c r="V20" t="n">
@@ -25055,13 +25127,13 @@
       <c r="K21" t="n">
         <v>30</v>
       </c>
-      <c r="L21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" t="b">
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="n">
         <v>1</v>
       </c>
       <c r="O21" t="inlineStr">
@@ -25069,22 +25141,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="b">
-        <v>0</v>
-      </c>
-      <c r="R21" t="inlineStr"/>
+      <c r="P21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S21" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T21" t="b">
-        <v>0</v>
-      </c>
-      <c r="U21" t="b">
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
         <v>0</v>
       </c>
       <c r="V21" t="n">
@@ -26252,13 +26328,13 @@
       <c r="K22" t="n">
         <v>22</v>
       </c>
-      <c r="L22" t="b">
-        <v>0</v>
-      </c>
-      <c r="M22" t="b">
-        <v>1</v>
-      </c>
-      <c r="N22" t="b">
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" t="n">
         <v>1</v>
       </c>
       <c r="O22" t="inlineStr">
@@ -26266,22 +26342,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P22" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="b">
-        <v>0</v>
-      </c>
-      <c r="R22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S22" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T22" t="b">
-        <v>0</v>
-      </c>
-      <c r="U22" t="b">
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
         <v>0</v>
       </c>
       <c r="V22" t="n">
@@ -27449,13 +27529,13 @@
       <c r="K23" t="n">
         <v>23</v>
       </c>
-      <c r="L23" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N23" t="b">
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" t="n">
         <v>1</v>
       </c>
       <c r="O23" t="inlineStr">
@@ -27463,22 +27543,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P23" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q23" t="b">
-        <v>0</v>
-      </c>
-      <c r="R23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T23" t="b">
-        <v>0</v>
-      </c>
-      <c r="U23" t="b">
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
         <v>0</v>
       </c>
       <c r="V23" t="n">
@@ -28646,13 +28730,13 @@
       <c r="K24" t="n">
         <v>19</v>
       </c>
-      <c r="L24" t="b">
-        <v>0</v>
-      </c>
-      <c r="M24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N24" t="b">
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
         <v>1</v>
       </c>
       <c r="O24" t="inlineStr">
@@ -28660,22 +28744,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P24" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q24" t="b">
-        <v>0</v>
-      </c>
-      <c r="R24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S24" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T24" t="b">
-        <v>0</v>
-      </c>
-      <c r="U24" t="b">
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="n">
@@ -29843,13 +29931,13 @@
       <c r="K25" t="n">
         <v>24</v>
       </c>
-      <c r="L25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M25" t="b">
-        <v>1</v>
-      </c>
-      <c r="N25" t="b">
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" t="n">
         <v>1</v>
       </c>
       <c r="O25" t="inlineStr">
@@ -29857,22 +29945,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P25" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="b">
-        <v>0</v>
-      </c>
-      <c r="R25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S25" t="inlineStr">
         <is>
           <t>Desarrollador</t>
         </is>
       </c>
-      <c r="T25" t="b">
-        <v>0</v>
-      </c>
-      <c r="U25" t="b">
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
         <v>0</v>
       </c>
       <c r="V25" t="n">
@@ -31040,13 +31132,13 @@
       <c r="K26" t="n">
         <v>23</v>
       </c>
-      <c r="L26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M26" t="b">
-        <v>1</v>
-      </c>
-      <c r="N26" t="b">
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" t="n">
         <v>1</v>
       </c>
       <c r="O26" t="inlineStr">
@@ -31054,22 +31146,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P26" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q26" t="b">
-        <v>0</v>
-      </c>
-      <c r="R26" t="inlineStr"/>
+      <c r="P26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S26" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T26" t="b">
-        <v>0</v>
-      </c>
-      <c r="U26" t="b">
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
         <v>0</v>
       </c>
       <c r="V26" t="n">
@@ -32237,13 +32333,13 @@
       <c r="K27" t="n">
         <v>24</v>
       </c>
-      <c r="L27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M27" t="b">
-        <v>1</v>
-      </c>
-      <c r="N27" t="b">
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" t="n">
         <v>1</v>
       </c>
       <c r="O27" t="inlineStr">
@@ -32251,22 +32347,26 @@
           <t>M</t>
         </is>
       </c>
-      <c r="P27" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q27" t="b">
-        <v>0</v>
-      </c>
-      <c r="R27" t="inlineStr"/>
+      <c r="P27" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T27" t="b">
-        <v>1</v>
-      </c>
-      <c r="U27" t="b">
+      <c r="T27" t="n">
+        <v>1</v>
+      </c>
+      <c r="U27" t="n">
         <v>0</v>
       </c>
       <c r="V27" t="n">
@@ -33434,13 +33534,13 @@
       <c r="K28" t="n">
         <v>23</v>
       </c>
-      <c r="L28" t="b">
-        <v>1</v>
-      </c>
-      <c r="M28" t="b">
-        <v>1</v>
-      </c>
-      <c r="N28" t="b">
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" t="n">
         <v>1</v>
       </c>
       <c r="O28" t="inlineStr">
@@ -33448,22 +33548,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P28" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q28" t="b">
-        <v>0</v>
-      </c>
-      <c r="R28" t="inlineStr"/>
+      <c r="P28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S28" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T28" t="b">
-        <v>0</v>
-      </c>
-      <c r="U28" t="b">
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
         <v>0</v>
       </c>
       <c r="V28" t="n">
@@ -34631,13 +34735,13 @@
       <c r="K29" t="n">
         <v>26</v>
       </c>
-      <c r="L29" t="b">
-        <v>1</v>
-      </c>
-      <c r="M29" t="b">
-        <v>1</v>
-      </c>
-      <c r="N29" t="b">
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M29" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" t="n">
         <v>1</v>
       </c>
       <c r="O29" t="inlineStr">
@@ -34645,22 +34749,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P29" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q29" t="b">
-        <v>0</v>
-      </c>
-      <c r="R29" t="inlineStr"/>
+      <c r="P29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S29" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T29" t="b">
-        <v>0</v>
-      </c>
-      <c r="U29" t="b">
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="n">
         <v>0</v>
       </c>
       <c r="V29" t="n">
@@ -35828,13 +35936,13 @@
       <c r="K30" t="n">
         <v>23</v>
       </c>
-      <c r="L30" t="b">
-        <v>0</v>
-      </c>
-      <c r="M30" t="b">
-        <v>0</v>
-      </c>
-      <c r="N30" t="b">
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
         <v>1</v>
       </c>
       <c r="O30" t="inlineStr">
@@ -35842,22 +35950,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P30" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R30" t="inlineStr"/>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S30" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U30" t="b">
+      <c r="T30" t="n">
+        <v>1</v>
+      </c>
+      <c r="U30" t="n">
         <v>0</v>
       </c>
       <c r="V30" t="n">
@@ -37025,13 +37137,13 @@
       <c r="K31" t="n">
         <v>23</v>
       </c>
-      <c r="L31" t="b">
-        <v>1</v>
-      </c>
-      <c r="M31" t="b">
-        <v>1</v>
-      </c>
-      <c r="N31" t="b">
+      <c r="L31" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" t="n">
         <v>1</v>
       </c>
       <c r="O31" t="inlineStr">
@@ -37039,22 +37151,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P31" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q31" t="b">
-        <v>0</v>
-      </c>
-      <c r="R31" t="inlineStr"/>
+      <c r="P31" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S31" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T31" t="b">
-        <v>0</v>
-      </c>
-      <c r="U31" t="b">
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
         <v>0</v>
       </c>
       <c r="V31" t="n">
@@ -38222,13 +38338,13 @@
       <c r="K32" t="n">
         <v>23</v>
       </c>
-      <c r="L32" t="b">
-        <v>1</v>
-      </c>
-      <c r="M32" t="b">
-        <v>1</v>
-      </c>
-      <c r="N32" t="b">
+      <c r="L32" t="n">
+        <v>1</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1</v>
+      </c>
+      <c r="N32" t="n">
         <v>1</v>
       </c>
       <c r="O32" t="inlineStr">
@@ -38236,22 +38352,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P32" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q32" t="b">
-        <v>0</v>
-      </c>
-      <c r="R32" t="inlineStr"/>
+      <c r="P32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr">
         <is>
           <t>Desempleado</t>
         </is>
       </c>
-      <c r="T32" t="b">
-        <v>0</v>
-      </c>
-      <c r="U32" t="b">
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
         <v>0</v>
       </c>
       <c r="V32" t="n">
@@ -39419,13 +39539,13 @@
       <c r="K33" t="n">
         <v>23</v>
       </c>
-      <c r="L33" t="b">
-        <v>0</v>
-      </c>
-      <c r="M33" t="b">
-        <v>1</v>
-      </c>
-      <c r="N33" t="b">
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" t="n">
         <v>1</v>
       </c>
       <c r="O33" t="inlineStr">
@@ -39433,22 +39553,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P33" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q33" t="b">
-        <v>0</v>
-      </c>
-      <c r="R33" t="inlineStr"/>
+      <c r="P33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S33" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T33" t="b">
-        <v>0</v>
-      </c>
-      <c r="U33" t="b">
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
         <v>0</v>
       </c>
       <c r="V33" t="n">
@@ -40616,13 +40740,13 @@
       <c r="K34" t="n">
         <v>24</v>
       </c>
-      <c r="L34" t="b">
-        <v>1</v>
-      </c>
-      <c r="M34" t="b">
-        <v>0</v>
-      </c>
-      <c r="N34" t="b">
+      <c r="L34" t="n">
+        <v>1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
         <v>1</v>
       </c>
       <c r="O34" t="inlineStr">
@@ -40630,22 +40754,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P34" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q34" t="b">
-        <v>0</v>
-      </c>
-      <c r="R34" t="inlineStr"/>
+      <c r="P34" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S34" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T34" t="b">
-        <v>0</v>
-      </c>
-      <c r="U34" t="b">
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
         <v>0</v>
       </c>
       <c r="V34" t="n">
@@ -41813,13 +41941,13 @@
       <c r="K35" t="n">
         <v>22</v>
       </c>
-      <c r="L35" t="b">
-        <v>1</v>
-      </c>
-      <c r="M35" t="b">
-        <v>1</v>
-      </c>
-      <c r="N35" t="b">
+      <c r="L35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
         <v>1</v>
       </c>
       <c r="O35" t="inlineStr">
@@ -41827,22 +41955,26 @@
           <t>J</t>
         </is>
       </c>
-      <c r="P35" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q35" t="b">
-        <v>0</v>
-      </c>
-      <c r="R35" t="inlineStr"/>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S35" t="inlineStr">
         <is>
           <t>Desempleado</t>
         </is>
       </c>
-      <c r="T35" t="b">
-        <v>0</v>
-      </c>
-      <c r="U35" t="b">
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
         <v>0</v>
       </c>
       <c r="V35" t="n">
@@ -43010,13 +43142,13 @@
       <c r="K36" t="n">
         <v>21</v>
       </c>
-      <c r="L36" t="b">
-        <v>0</v>
-      </c>
-      <c r="M36" t="b">
-        <v>1</v>
-      </c>
-      <c r="N36" t="b">
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
         <v>1</v>
       </c>
       <c r="O36" t="inlineStr">
@@ -43024,22 +43156,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P36" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q36" t="b">
-        <v>0</v>
-      </c>
-      <c r="R36" t="inlineStr"/>
+      <c r="P36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S36" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T36" t="b">
-        <v>0</v>
-      </c>
-      <c r="U36" t="b">
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="n">
         <v>0</v>
       </c>
       <c r="V36" t="n">
@@ -44207,13 +44343,13 @@
       <c r="K37" t="n">
         <v>21</v>
       </c>
-      <c r="L37" t="b">
-        <v>0</v>
-      </c>
-      <c r="M37" t="b">
-        <v>1</v>
-      </c>
-      <c r="N37" t="b">
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N37" t="n">
         <v>1</v>
       </c>
       <c r="O37" t="inlineStr">
@@ -44221,22 +44357,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P37" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q37" t="b">
-        <v>0</v>
-      </c>
-      <c r="R37" t="inlineStr"/>
+      <c r="P37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T37" t="b">
-        <v>0</v>
-      </c>
-      <c r="U37" t="b">
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
         <v>0</v>
       </c>
       <c r="V37" t="n">
@@ -45404,13 +45544,13 @@
       <c r="K38" t="n">
         <v>21</v>
       </c>
-      <c r="L38" t="b">
-        <v>0</v>
-      </c>
-      <c r="M38" t="b">
-        <v>1</v>
-      </c>
-      <c r="N38" t="b">
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N38" t="n">
         <v>1</v>
       </c>
       <c r="O38" t="inlineStr">
@@ -45418,22 +45558,26 @@
           <t>M</t>
         </is>
       </c>
-      <c r="P38" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q38" t="b">
-        <v>0</v>
-      </c>
-      <c r="R38" t="inlineStr"/>
+      <c r="P38" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S38" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T38" t="b">
-        <v>0</v>
-      </c>
-      <c r="U38" t="b">
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
         <v>0</v>
       </c>
       <c r="V38" t="n">
@@ -46601,13 +46745,13 @@
       <c r="K39" t="n">
         <v>23</v>
       </c>
-      <c r="L39" t="b">
-        <v>0</v>
-      </c>
-      <c r="M39" t="b">
-        <v>1</v>
-      </c>
-      <c r="N39" t="b">
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" t="n">
         <v>1</v>
       </c>
       <c r="O39" t="inlineStr">
@@ -46615,22 +46759,26 @@
           <t>S</t>
         </is>
       </c>
-      <c r="P39" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q39" t="b">
-        <v>0</v>
-      </c>
-      <c r="R39" t="inlineStr"/>
+      <c r="P39" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S39" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T39" t="b">
-        <v>0</v>
-      </c>
-      <c r="U39" t="b">
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
         <v>0</v>
       </c>
       <c r="V39" t="n">
@@ -47798,13 +47946,13 @@
       <c r="K40" t="n">
         <v>23</v>
       </c>
-      <c r="L40" t="b">
-        <v>1</v>
-      </c>
-      <c r="M40" t="b">
-        <v>1</v>
-      </c>
-      <c r="N40" t="b">
+      <c r="L40" t="n">
+        <v>1</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1</v>
+      </c>
+      <c r="N40" t="n">
         <v>1</v>
       </c>
       <c r="O40" t="inlineStr">
@@ -47812,22 +47960,26 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P40" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q40" t="b">
-        <v>0</v>
-      </c>
-      <c r="R40" t="inlineStr"/>
+      <c r="P40" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S40" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T40" t="b">
-        <v>0</v>
-      </c>
-      <c r="U40" t="b">
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="n">
         <v>0</v>
       </c>
       <c r="V40" t="n">
@@ -48995,13 +49147,13 @@
       <c r="K41" t="n">
         <v>24</v>
       </c>
-      <c r="L41" t="b">
-        <v>1</v>
-      </c>
-      <c r="M41" t="b">
-        <v>1</v>
-      </c>
-      <c r="N41" t="b">
+      <c r="L41" t="n">
+        <v>1</v>
+      </c>
+      <c r="M41" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" t="n">
         <v>1</v>
       </c>
       <c r="O41" t="inlineStr">
@@ -49009,10 +49161,10 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P41" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q41" t="b">
+      <c r="P41" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="n">
         <v>0</v>
       </c>
       <c r="R41" t="inlineStr"/>
@@ -49021,10 +49173,10 @@
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T41" t="b">
-        <v>1</v>
-      </c>
-      <c r="U41" t="b">
+      <c r="T41" t="n">
+        <v>1</v>
+      </c>
+      <c r="U41" t="n">
         <v>0</v>
       </c>
       <c r="V41" t="n">
@@ -50192,13 +50344,13 @@
       <c r="K42" t="n">
         <v>24</v>
       </c>
-      <c r="L42" t="b">
-        <v>0</v>
-      </c>
-      <c r="M42" t="b">
-        <v>1</v>
-      </c>
-      <c r="N42" t="b">
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>1</v>
+      </c>
+      <c r="N42" t="n">
         <v>1</v>
       </c>
       <c r="O42" t="inlineStr">
@@ -50206,10 +50358,10 @@
           <t>A</t>
         </is>
       </c>
-      <c r="P42" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q42" t="b">
+      <c r="P42" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q42" t="n">
         <v>0</v>
       </c>
       <c r="R42" t="inlineStr"/>
@@ -50218,10 +50370,10 @@
           <t>Contratista Ingeniero Electrónico</t>
         </is>
       </c>
-      <c r="T42" t="b">
-        <v>0</v>
-      </c>
-      <c r="U42" t="b">
+      <c r="T42" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" t="n">
         <v>0</v>
       </c>
       <c r="V42" t="n">
@@ -51389,13 +51541,13 @@
       <c r="K43" t="n">
         <v>17</v>
       </c>
-      <c r="L43" t="b">
-        <v>0</v>
-      </c>
-      <c r="M43" t="b">
-        <v>1</v>
-      </c>
-      <c r="N43" t="b">
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>1</v>
+      </c>
+      <c r="N43" t="n">
         <v>1</v>
       </c>
       <c r="O43" t="inlineStr">
@@ -51403,22 +51555,26 @@
           <t>P</t>
         </is>
       </c>
-      <c r="P43" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q43" t="b">
-        <v>0</v>
-      </c>
-      <c r="R43" t="inlineStr"/>
+      <c r="P43" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>No aplica</t>
+        </is>
+      </c>
       <c r="S43" t="inlineStr">
         <is>
           <t>Estudiante</t>
         </is>
       </c>
-      <c r="T43" t="b">
-        <v>0</v>
-      </c>
-      <c r="U43" t="b">
+      <c r="T43" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" t="n">
         <v>0</v>
       </c>
       <c r="V43" t="n">

</xml_diff>